<commit_message>
Edits to all app
</commit_message>
<xml_diff>
--- a/data/mock_database.xlsx
+++ b/data/mock_database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmbro\Documents\Projects\KindredConnect\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmbro\Documents\Projects\kc_open\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BAE276-6703-4BEF-8738-15E48607E032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6009D318-86FA-442B-8D56-B9F40BDD4AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{64B6D4B8-102B-46F3-9450-EFE968D2A28C}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="84">
   <si>
     <t>Id</t>
   </si>
@@ -290,6 +290,9 @@
   </si>
   <si>
     <t>andrea.brock</t>
+  </si>
+  <si>
+    <t>AccumulatedDonationValue</t>
   </si>
 </sst>
 </file>
@@ -684,9 +687,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE6222B-08F6-479E-85D6-4BBCDB6101D6}">
-  <dimension ref="A1:Y6"/>
+  <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="Y7" sqref="Y7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -708,10 +713,11 @@
     <col min="22" max="22" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="22" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.85546875" style="3" customWidth="1"/>
+    <col min="25" max="25" width="22" customWidth="1"/>
+    <col min="26" max="26" width="12.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -785,10 +791,13 @@
         <v>18</v>
       </c>
       <c r="Y1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -855,11 +864,14 @@
       <c r="W2" t="s">
         <v>24</v>
       </c>
-      <c r="Y2" s="3">
-        <v>45814</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y2">
+        <v>800</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>45814</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -923,11 +935,14 @@
       <c r="U3" t="s">
         <v>81</v>
       </c>
-      <c r="Y3" s="3">
-        <v>45814</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y3">
+        <v>9000</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>45814</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -967,11 +982,14 @@
       <c r="T4" t="s">
         <v>82</v>
       </c>
-      <c r="Y4" s="3">
-        <v>45814</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y4">
+        <v>324</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>45814</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1026,11 +1044,14 @@
       <c r="X5">
         <v>8005543678</v>
       </c>
-      <c r="Y5" s="3">
-        <v>45814</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y5">
+        <v>56.32</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>45814</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1070,7 +1091,10 @@
       <c r="T6" t="s">
         <v>82</v>
       </c>
-      <c r="Y6" s="3">
+      <c r="Y6">
+        <v>123.45</v>
+      </c>
+      <c r="Z6" s="3">
         <v>45814</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement add new donors
</commit_message>
<xml_diff>
--- a/data/mock_database.xlsx
+++ b/data/mock_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmbro\Documents\Projects\kc_open\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6009D318-86FA-442B-8D56-B9F40BDD4AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB4C385-297B-423E-A65B-729BDEC21760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{64B6D4B8-102B-46F3-9450-EFE968D2A28C}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="105">
   <si>
     <t>Id</t>
   </si>
@@ -61,15 +61,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>PhoneType</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>SpouseId</t>
   </si>
   <si>
@@ -109,9 +100,6 @@
     <t>Individual</t>
   </si>
   <si>
-    <t>gabnoia@gmail.com</t>
-  </si>
-  <si>
     <t>andbrock</t>
   </si>
   <si>
@@ -124,12 +112,6 @@
     <t>Mrs.</t>
   </si>
   <si>
-    <t>Alberto</t>
-  </si>
-  <si>
-    <t>Roberto</t>
-  </si>
-  <si>
     <t>Residential</t>
   </si>
   <si>
@@ -160,9 +142,6 @@
     <t>Retail</t>
   </si>
   <si>
-    <t>Paul</t>
-  </si>
-  <si>
     <t>Silvanian</t>
   </si>
   <si>
@@ -193,9 +172,6 @@
     <t>Cash</t>
   </si>
   <si>
-    <t>Solange</t>
-  </si>
-  <si>
     <t>Check</t>
   </si>
   <si>
@@ -238,15 +214,6 @@
     <t>Other</t>
   </si>
   <si>
-    <t>debinha145@gmail.com</t>
-  </si>
-  <si>
-    <t>Delta Marin</t>
-  </si>
-  <si>
-    <t>Gilberto</t>
-  </si>
-  <si>
     <t>Madeiros</t>
   </si>
   <si>
@@ -256,24 +223,6 @@
     <t>Bach</t>
   </si>
   <si>
-    <t>Street</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>ZipCode</t>
-  </si>
-  <si>
-    <t>Calle A</t>
-  </si>
-  <si>
     <t>New Formation</t>
   </si>
   <si>
@@ -293,6 +242,120 @@
   </si>
   <si>
     <t>AccumulatedDonationValue</t>
+  </si>
+  <si>
+    <t>gibnoia@gmail.com</t>
+  </si>
+  <si>
+    <t>delmm145@gmail.com</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>Cel</t>
+  </si>
+  <si>
+    <t>PhoneType1</t>
+  </si>
+  <si>
+    <t>Phone1</t>
+  </si>
+  <si>
+    <t>PhoneType2</t>
+  </si>
+  <si>
+    <t>Phone2</t>
+  </si>
+  <si>
+    <t>Phone3</t>
+  </si>
+  <si>
+    <t>PhoneType3</t>
+  </si>
+  <si>
+    <t>Pinewoods</t>
+  </si>
+  <si>
+    <t>Email1</t>
+  </si>
+  <si>
+    <t>Email2</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>gibnoia@hotmail.com</t>
+  </si>
+  <si>
+    <t>Street1</t>
+  </si>
+  <si>
+    <t>City1</t>
+  </si>
+  <si>
+    <t>State1</t>
+  </si>
+  <si>
+    <t>Country1</t>
+  </si>
+  <si>
+    <t>ZipCode1</t>
+  </si>
+  <si>
+    <t>Street2</t>
+  </si>
+  <si>
+    <t>City2</t>
+  </si>
+  <si>
+    <t>State2</t>
+  </si>
+  <si>
+    <t>Country2</t>
+  </si>
+  <si>
+    <t>ZipCode2</t>
+  </si>
+  <si>
+    <t>Sandra</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Albert</t>
+  </si>
+  <si>
+    <t>Daniella</t>
+  </si>
+  <si>
+    <t>Roberts</t>
+  </si>
+  <si>
+    <t>Vancouver</t>
+  </si>
+  <si>
+    <t>British Columbia</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>V4L1D0</t>
+  </si>
+  <si>
+    <t>1008 N West Virginia</t>
+  </si>
+  <si>
+    <t>(999) 888-7777</t>
+  </si>
+  <si>
+    <t>CompanyWebsite</t>
+  </si>
+  <si>
+    <t>www.newsite.com</t>
   </si>
 </sst>
 </file>
@@ -687,427 +750,546 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE6222B-08F6-479E-85D6-4BBCDB6101D6}">
-  <dimension ref="A1:Z6"/>
+  <dimension ref="A1:AK6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Y7" sqref="Y7"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="26.28515625" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="22" customWidth="1"/>
-    <col min="26" max="26" width="12.85546875" style="3" customWidth="1"/>
+    <col min="8" max="12" width="12.7109375" customWidth="1"/>
+    <col min="13" max="13" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22" bestFit="1" customWidth="1"/>
+    <col min="19" max="24" width="22" customWidth="1"/>
+    <col min="25" max="29" width="26.28515625" customWidth="1"/>
+    <col min="31" max="31" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22" customWidth="1"/>
+    <col min="33" max="33" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.85546875" style="3" customWidth="1"/>
+    <col min="36" max="36" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" t="s">
+        <v>103</v>
+      </c>
+      <c r="T1" t="s">
+        <v>82</v>
+      </c>
+      <c r="U1" t="s">
+        <v>83</v>
+      </c>
+      <c r="V1" t="s">
+        <v>84</v>
+      </c>
+      <c r="W1" t="s">
+        <v>85</v>
+      </c>
+      <c r="X1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="AE1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="AF1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>71</v>
-      </c>
-      <c r="K1" t="s">
-        <v>72</v>
-      </c>
-      <c r="L1" t="s">
-        <v>73</v>
-      </c>
-      <c r="M1" t="s">
-        <v>74</v>
-      </c>
-      <c r="N1" t="s">
-        <v>75</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="AH1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" t="s">
+      <c r="AI1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AK1" t="s">
         <v>11</v>
       </c>
-      <c r="R1" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" t="s">
-        <v>13</v>
-      </c>
-      <c r="T1" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" t="s">
-        <v>15</v>
-      </c>
-      <c r="V1" t="s">
-        <v>16</v>
-      </c>
-      <c r="W1" t="s">
-        <v>17</v>
-      </c>
-      <c r="X1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" t="s">
+        <v>102</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="N2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q2" t="s">
         <v>20</v>
       </c>
-      <c r="H2">
-        <v>6045575524</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="T2" t="s">
         <v>77</v>
       </c>
-      <c r="L2" t="s">
-        <v>78</v>
-      </c>
-      <c r="M2" t="s">
-        <v>79</v>
-      </c>
-      <c r="N2">
-        <v>234445</v>
-      </c>
-      <c r="O2">
+      <c r="U2" t="s">
+        <v>60</v>
+      </c>
+      <c r="V2" t="s">
+        <v>61</v>
+      </c>
+      <c r="W2" t="s">
+        <v>62</v>
+      </c>
+      <c r="X2" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD2">
         <v>2</v>
       </c>
-      <c r="P2">
+      <c r="AE2">
         <v>1</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="AF2">
+        <v>800</v>
+      </c>
+      <c r="AG2" s="3">
         <v>45778</v>
       </c>
-      <c r="R2" t="s">
-        <v>82</v>
-      </c>
-      <c r="S2" s="3">
+      <c r="AH2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI2" s="3">
+        <v>45814</v>
+      </c>
+      <c r="AJ2" s="3">
         <v>45778</v>
       </c>
-      <c r="T2" t="s">
-        <v>82</v>
-      </c>
-      <c r="U2" t="s">
-        <v>80</v>
-      </c>
-      <c r="W2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y2">
-        <v>800</v>
-      </c>
-      <c r="Z2" s="3">
-        <v>45814</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AK2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" t="s">
+        <v>102</v>
+      </c>
+      <c r="K3" t="s">
+        <v>80</v>
+      </c>
+      <c r="L3" t="s">
+        <v>102</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3">
-        <v>7788596857</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="N3" s="2"/>
+      <c r="O3" t="s">
+        <v>64</v>
+      </c>
+      <c r="T3" t="s">
+        <v>77</v>
+      </c>
+      <c r="U3" t="s">
+        <v>60</v>
+      </c>
+      <c r="V3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W3" t="s">
+        <v>62</v>
+      </c>
+      <c r="X3" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>2</v>
+      </c>
+      <c r="AF3">
+        <v>9000</v>
+      </c>
+      <c r="AG3" s="3">
+        <v>45780</v>
+      </c>
+      <c r="AH3" t="s">
         <v>65</v>
       </c>
-      <c r="J3" t="s">
-        <v>76</v>
-      </c>
-      <c r="K3" t="s">
-        <v>77</v>
-      </c>
-      <c r="L3" t="s">
-        <v>78</v>
-      </c>
-      <c r="M3" t="s">
-        <v>79</v>
-      </c>
-      <c r="N3">
-        <v>234445</v>
-      </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="3">
+      <c r="AI3" s="3">
+        <v>45814</v>
+      </c>
+      <c r="AJ3" s="3">
         <v>45780</v>
       </c>
-      <c r="R3" t="s">
-        <v>82</v>
-      </c>
-      <c r="S3" s="3">
-        <v>45780</v>
-      </c>
-      <c r="T3" t="s">
-        <v>82</v>
-      </c>
-      <c r="U3" t="s">
-        <v>81</v>
-      </c>
-      <c r="Y3">
-        <v>9000</v>
-      </c>
-      <c r="Z3" s="3">
-        <v>45814</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AK3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s">
-        <v>28</v>
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>94</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4">
-        <v>6040000000</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="P4">
+        <v>70</v>
+      </c>
+      <c r="H4" t="s">
+        <v>102</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="2"/>
+      <c r="AE4">
         <v>3</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="AF4">
+        <v>324</v>
+      </c>
+      <c r="AG4" s="3">
         <v>45807</v>
       </c>
-      <c r="R4" t="s">
-        <v>82</v>
-      </c>
-      <c r="S4" s="3">
+      <c r="AH4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI4" s="3">
+        <v>45814</v>
+      </c>
+      <c r="AJ4" s="3">
         <v>45809</v>
       </c>
-      <c r="T4" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y4">
-        <v>324</v>
-      </c>
-      <c r="Z4" s="3">
-        <v>45814</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AK4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" t="s">
+        <v>102</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" s="2"/>
+      <c r="O5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5" t="s">
         <v>31</v>
       </c>
-      <c r="C5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="Q5" t="s">
         <v>32</v>
       </c>
-      <c r="E5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5">
-        <v>6051111111</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P5">
+      <c r="R5" t="s">
+        <v>102</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="T5" t="s">
+        <v>101</v>
+      </c>
+      <c r="U5" t="s">
+        <v>97</v>
+      </c>
+      <c r="V5" t="s">
+        <v>98</v>
+      </c>
+      <c r="W5" t="s">
+        <v>99</v>
+      </c>
+      <c r="X5" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE5">
         <v>5</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="AF5">
+        <v>56.32</v>
+      </c>
+      <c r="AG5" s="3">
         <v>45770</v>
       </c>
-      <c r="R5" t="s">
-        <v>82</v>
-      </c>
-      <c r="S5" s="3">
+      <c r="AH5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI5" s="3">
+        <v>45814</v>
+      </c>
+      <c r="AJ5" s="3">
         <v>45777</v>
       </c>
-      <c r="T5" t="s">
-        <v>82</v>
-      </c>
-      <c r="U5" t="s">
-        <v>36</v>
-      </c>
-      <c r="V5" t="s">
-        <v>37</v>
-      </c>
-      <c r="W5" t="s">
-        <v>38</v>
-      </c>
-      <c r="X5">
-        <v>8005543678</v>
-      </c>
-      <c r="Y5">
-        <v>56.32</v>
-      </c>
-      <c r="Z5" s="3">
-        <v>45814</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AK5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P6">
+        <v>69</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" s="2"/>
+      <c r="AE6">
         <v>6</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="AF6">
+        <v>123.45</v>
+      </c>
+      <c r="AG6" s="3">
         <v>45762</v>
       </c>
-      <c r="R6" t="s">
-        <v>82</v>
-      </c>
-      <c r="S6" s="3">
+      <c r="AH6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI6" s="3">
+        <v>45814</v>
+      </c>
+      <c r="AJ6" s="3">
         <v>45762</v>
       </c>
-      <c r="T6" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y6">
-        <v>123.45</v>
-      </c>
-      <c r="Z6" s="3">
-        <v>45814</v>
+      <c r="AK6" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{E754FF2B-653B-42E7-8E64-9061E5F0830C}"/>
-    <hyperlink ref="I3" r:id="rId2" xr:uid="{04A7ACCF-B351-4066-8D59-857330D39D12}"/>
-    <hyperlink ref="I4" r:id="rId3" xr:uid="{EA59449C-AE49-48A7-97DC-6AFA04614089}"/>
-    <hyperlink ref="I5" r:id="rId4" xr:uid="{BB373B3D-CCBE-41B0-8D14-5DB5C0C7F999}"/>
-    <hyperlink ref="I6" r:id="rId5" xr:uid="{CB7E9D17-1872-495F-86BB-47A30CC75446}"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{E754FF2B-653B-42E7-8E64-9061E5F0830C}"/>
+    <hyperlink ref="M3" r:id="rId2" xr:uid="{04A7ACCF-B351-4066-8D59-857330D39D12}"/>
+    <hyperlink ref="M4" r:id="rId3" xr:uid="{EA59449C-AE49-48A7-97DC-6AFA04614089}"/>
+    <hyperlink ref="M5" r:id="rId4" xr:uid="{BB373B3D-CCBE-41B0-8D14-5DB5C0C7F999}"/>
+    <hyperlink ref="M6" r:id="rId5" xr:uid="{CB7E9D17-1872-495F-86BB-47A30CC75446}"/>
+    <hyperlink ref="N2" r:id="rId6" xr:uid="{0440F225-865C-4D53-9146-E47D482EF42D}"/>
+    <hyperlink ref="S5" r:id="rId7" xr:uid="{2F542E50-2FE9-494F-A334-FA61F7B3AF8A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -1115,7 +1297,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054FAB06-9A5E-4B1A-8C4C-B35850004FA0}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1131,28 +1315,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1172,13 +1356,13 @@
         <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G2" s="3">
         <v>45791</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I2" s="3">
         <v>45814</v>
@@ -1204,7 +1388,7 @@
         <v>45791</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I3" s="3">
         <v>45814</v>
@@ -1227,13 +1411,13 @@
         <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G4" s="3">
         <v>45809</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I4" s="3">
         <v>45814</v>
@@ -1256,13 +1440,13 @@
         <v>100</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G5" s="3">
         <v>45767</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I5" s="3">
         <v>45814</v>
@@ -1285,13 +1469,13 @@
         <v>500</v>
       </c>
       <c r="F6" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G6" s="3">
         <v>45770</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I6" s="3">
         <v>45814</v>
@@ -1314,13 +1498,13 @@
         <v>350</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G7" s="3">
         <v>45770</v>
       </c>
       <c r="H7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I7" s="3">
         <v>45814</v>
@@ -1355,37 +1539,37 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
         <v>52</v>
       </c>
-      <c r="C1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" t="s">
-        <v>60</v>
-      </c>
       <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
       <c r="L1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1393,7 +1577,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C2" s="3">
         <v>45789</v>
@@ -1405,7 +1589,7 @@
         <v>45872</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G2" s="4">
         <v>1</v>
@@ -1414,13 +1598,13 @@
         <v>45787</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J2" s="3">
         <v>45788</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="L2" s="3">
         <v>45814</v>
@@ -1431,7 +1615,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C3" s="3">
         <v>45809</v>
@@ -1443,7 +1627,7 @@
         <v>45840</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G3" s="4">
         <v>1</v>
@@ -1452,13 +1636,13 @@
         <v>45805</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J3" s="3">
         <v>45805</v>
       </c>
       <c r="K3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="L3" s="3">
         <v>45814</v>
@@ -1469,7 +1653,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C4" s="3">
         <v>45748</v>
@@ -1481,7 +1665,7 @@
         <v>45778</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -1490,13 +1674,13 @@
         <v>45731</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J4" s="3">
         <v>45731</v>
       </c>
       <c r="K4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="L4" s="3">
         <v>45814</v>
@@ -1507,7 +1691,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C5" s="3">
         <v>45658</v>
@@ -1522,13 +1706,13 @@
         <v>45657</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J5" s="3">
         <v>45657</v>
       </c>
       <c r="K5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="L5" s="3">
         <v>45814</v>
@@ -1558,7 +1742,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1566,7 +1750,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3">
         <v>45814</v>
@@ -1577,7 +1761,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3">
         <v>45814</v>
@@ -1588,7 +1772,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C4" s="3">
         <v>45814</v>
@@ -1599,7 +1783,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C5" s="3">
         <v>45814</v>
@@ -1632,7 +1816,7 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1640,7 +1824,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3">
         <v>45814</v>
@@ -1651,7 +1835,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3">
         <v>45814</v>
@@ -1682,7 +1866,7 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1690,7 +1874,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3">
         <v>45814</v>
@@ -1701,7 +1885,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3">
         <v>45814</v>
@@ -1712,7 +1896,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C4" s="3">
         <v>45814</v>

</xml_diff>

<commit_message>
Add server logic to new event and new donation
</commit_message>
<xml_diff>
--- a/data/mock_database.xlsx
+++ b/data/mock_database.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmbro\Documents\Projects\kc_open\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB4C385-297B-423E-A65B-729BDEC21760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF900CB-8D30-409C-80BF-C8881FA756ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{64B6D4B8-102B-46F3-9450-EFE968D2A28C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{64B6D4B8-102B-46F3-9450-EFE968D2A28C}"/>
   </bookViews>
   <sheets>
     <sheet name="Donor" sheetId="1" r:id="rId1"/>
     <sheet name="Donation" sheetId="2" r:id="rId2"/>
-    <sheet name="Raffle" sheetId="3" r:id="rId3"/>
+    <sheet name="Events" sheetId="3" r:id="rId3"/>
     <sheet name="Title" sheetId="4" r:id="rId4"/>
     <sheet name="DonorType" sheetId="5" r:id="rId5"/>
     <sheet name="PhoneType" sheetId="6" r:id="rId6"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="107">
   <si>
     <t>Id</t>
   </si>
@@ -356,6 +356,12 @@
   </si>
   <si>
     <t>www.newsite.com</t>
+  </si>
+  <si>
+    <t>Type 1</t>
+  </si>
+  <si>
+    <t>Type 2</t>
   </si>
 </sst>
 </file>
@@ -752,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE6222B-08F6-479E-85D6-4BBCDB6101D6}">
   <dimension ref="A1:AK6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,22 +1301,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054FAB06-9A5E-4B1A-8C4C-B35850004FA0}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1329,17 +1336,20 @@
       <c r="F1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1358,17 +1368,20 @@
       <c r="F2" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" s="3">
         <v>45791</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="3">
-        <v>45814</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="3">
+        <v>45814</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1384,17 +1397,17 @@
       <c r="E3">
         <v>75</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>45791</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="3">
-        <v>45814</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="3">
+        <v>45814</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1413,17 +1426,17 @@
       <c r="F4" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>45809</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="3">
-        <v>45814</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="3">
+        <v>45814</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1442,17 +1455,20 @@
       <c r="F5" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H5" s="3">
         <v>45767</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="3">
-        <v>45814</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="3">
+        <v>45814</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1471,17 +1487,17 @@
       <c r="F6" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="3">
         <v>45770</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="3">
-        <v>45814</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="3">
+        <v>45814</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1500,13 +1516,13 @@
       <c r="F7" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>45770</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="3">
+      <c r="J7" s="3">
         <v>45814</v>
       </c>
     </row>
@@ -1519,7 +1535,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA0474F5-D1A6-4EB4-9790-6BFEFCFA308E}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1850,7 +1868,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0781E15-A7DC-494E-BE45-809C8FE9208D}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Minor fixes to UI
</commit_message>
<xml_diff>
--- a/data/mock_database.xlsx
+++ b/data/mock_database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmbro\Documents\Projects\kc_open\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF900CB-8D30-409C-80BF-C8881FA756ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053CE733-F2F0-4B89-A66C-2309F9A1FDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{64B6D4B8-102B-46F3-9450-EFE968D2A28C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{64B6D4B8-102B-46F3-9450-EFE968D2A28C}"/>
   </bookViews>
   <sheets>
     <sheet name="Donor" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="108">
   <si>
     <t>Id</t>
   </si>
@@ -362,6 +362,9 @@
   </si>
   <si>
     <t>Type 2</t>
+  </si>
+  <si>
+    <t>Not Related</t>
   </si>
 </sst>
 </file>
@@ -1533,10 +1536,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA0474F5-D1A6-4EB4-9790-6BFEFCFA308E}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1595,54 +1598,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="3">
-        <v>45789</v>
-      </c>
-      <c r="D2" s="3">
-        <v>45869</v>
-      </c>
-      <c r="E2" s="3">
-        <v>45872</v>
-      </c>
-      <c r="F2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="4">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3">
-        <v>45787</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="3">
-        <v>45788</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="3">
-        <v>45814</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="J2"/>
+      <c r="L2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C3" s="3">
-        <v>45809</v>
+        <v>45789</v>
       </c>
       <c r="D3" s="3">
-        <v>45838</v>
+        <v>45869</v>
       </c>
       <c r="E3" s="3">
-        <v>45840</v>
+        <v>45872</v>
       </c>
       <c r="F3" t="s">
         <v>53</v>
@@ -1651,13 +1631,13 @@
         <v>1</v>
       </c>
       <c r="H3" s="3">
-        <v>45805</v>
+        <v>45787</v>
       </c>
       <c r="I3" t="s">
         <v>19</v>
       </c>
       <c r="J3" s="3">
-        <v>45805</v>
+        <v>45788</v>
       </c>
       <c r="K3" t="s">
         <v>19</v>
@@ -1671,31 +1651,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C4" s="3">
-        <v>45748</v>
+        <v>45809</v>
       </c>
       <c r="D4" s="3">
-        <v>45777</v>
+        <v>45838</v>
       </c>
       <c r="E4" s="3">
-        <v>45778</v>
+        <v>45840</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="3">
-        <v>45731</v>
+        <v>45805</v>
       </c>
       <c r="I4" t="s">
         <v>19</v>
       </c>
       <c r="J4" s="3">
-        <v>45731</v>
+        <v>45805</v>
       </c>
       <c r="K4" t="s">
         <v>19</v>
@@ -1709,30 +1689,68 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C5" s="3">
-        <v>45658</v>
+        <v>45748</v>
       </c>
       <c r="D5" s="3">
-        <v>46022</v>
+        <v>45777</v>
+      </c>
+      <c r="E5" s="3">
+        <v>45778</v>
+      </c>
+      <c r="F5" t="s">
+        <v>51</v>
       </c>
       <c r="G5" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="3">
-        <v>45657</v>
+        <v>45731</v>
       </c>
       <c r="I5" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="3">
-        <v>45657</v>
+        <v>45731</v>
       </c>
       <c r="K5" t="s">
         <v>19</v>
       </c>
       <c r="L5" s="3">
+        <v>45814</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="3">
+        <v>45658</v>
+      </c>
+      <c r="D6" s="3">
+        <v>46022</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3">
+        <v>45657</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="3">
+        <v>45657</v>
+      </c>
+      <c r="K6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="3">
         <v>45814</v>
       </c>
     </row>
@@ -1868,7 +1886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0781E15-A7DC-494E-BE45-809C8FE9208D}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>

</xml_diff>